<commit_message>
ligne de config retirée
</commit_message>
<xml_diff>
--- a/notes_2019_2020.xlsx
+++ b/notes_2019_2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\Nouveau dossier (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\AS_INFO\matlab\projet\Projet_MathLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73C6A3C-B9D3-42E3-8D2D-3DF305786890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126D1D34-8A9B-41C3-9DDE-0F107B348D9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="39">
   <si>
     <t>D</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">C </t>
-  </si>
-  <si>
-    <t>b+</t>
   </si>
   <si>
     <t>Note Fin</t>
@@ -994,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,18 +1012,18 @@
     <col min="13" max="16" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="68"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="69">
         <v>43761</v>
       </c>
@@ -1047,7 +1044,7 @@
       <c r="K3" s="45"/>
       <c r="L3" s="46"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="47" t="s">
         <v>3</v>
       </c>
@@ -1067,7 +1064,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="52" t="s">
         <v>11</v>
@@ -1076,13 +1073,13 @@
         <v>14</v>
       </c>
       <c r="K4" s="54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L4" s="55" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="61">
         <v>1</v>
       </c>
@@ -1113,48 +1110,45 @@
       <c r="K5" s="60"/>
       <c r="L5" s="67"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="40">
+        <v>7</v>
+      </c>
+      <c r="L6" s="42"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="40">
-        <v>7</v>
-      </c>
-      <c r="L6" s="42"/>
-      <c r="M6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
-        <v>39</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>0</v>
@@ -1187,13 +1181,10 @@
         <v>8</v>
       </c>
       <c r="L7" s="42"/>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>0</v>
@@ -1226,15 +1217,12 @@
         <v>8</v>
       </c>
       <c r="L8" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>0</v>
@@ -1267,13 +1255,10 @@
         <v>9</v>
       </c>
       <c r="L9" s="42"/>
-      <c r="M9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>2</v>
@@ -1306,13 +1291,10 @@
         <v>11</v>
       </c>
       <c r="L10" s="42"/>
-      <c r="M10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>0</v>
@@ -1345,15 +1327,12 @@
         <v>9</v>
       </c>
       <c r="L11" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>1</v>
@@ -1386,13 +1365,10 @@
         <v>9</v>
       </c>
       <c r="L12" s="42"/>
-      <c r="M12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>1</v>
@@ -1425,15 +1401,12 @@
         <v>14</v>
       </c>
       <c r="L13" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>0</v>
@@ -1466,15 +1439,12 @@
         <v>9</v>
       </c>
       <c r="L14" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>0</v>
@@ -1507,15 +1477,12 @@
         <v>12</v>
       </c>
       <c r="L15" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>0</v>
@@ -1548,15 +1515,12 @@
         <v>7</v>
       </c>
       <c r="L16" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="M16">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>0</v>
@@ -1589,13 +1553,10 @@
         <v>9</v>
       </c>
       <c r="L17" s="42"/>
-      <c r="M17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>1</v>
@@ -1628,15 +1589,12 @@
         <v>17</v>
       </c>
       <c r="L18" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>0</v>
@@ -1669,13 +1627,10 @@
         <v>11</v>
       </c>
       <c r="L19" s="42"/>
-      <c r="M19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>2</v>
@@ -1708,15 +1663,12 @@
         <v>18</v>
       </c>
       <c r="L20" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>0</v>
@@ -1749,71 +1701,7 @@
         <v>7</v>
       </c>
       <c r="L21" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" t="s">
-        <v>6</v>
-      </c>
-      <c r="M26" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D27">
-        <v>5</v>
-      </c>
-      <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="F27">
-        <v>9</v>
-      </c>
-      <c r="G27">
-        <v>9</v>
-      </c>
-      <c r="H27">
-        <v>11</v>
-      </c>
-      <c r="I27">
-        <v>10</v>
-      </c>
-      <c r="J27">
-        <v>12</v>
-      </c>
-      <c r="K27">
-        <v>12</v>
-      </c>
-      <c r="L27">
-        <v>16</v>
-      </c>
-      <c r="M27">
-        <v>14</v>
-      </c>
-      <c r="N27">
-        <v>16</v>
-      </c>
-      <c r="O27">
-        <v>16</v>
-      </c>
-      <c r="P27">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1848,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12:E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>